<commit_message>
Right menu for actions work in progress
</commit_message>
<xml_diff>
--- a/src/main/resources/benchmarks.xlsx
+++ b/src/main/resources/benchmarks.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="88">
   <si>
     <t>known ticks</t>
   </si>
@@ -284,7 +284,13 @@
     <t>1.1.0</t>
   </si>
   <si>
-    <t>ParentA iterator to for cycle</t>
+    <t>SplittableRandom instead of MersenneTwisterFast</t>
+  </si>
+  <si>
+    <t>1.1.1</t>
+  </si>
+  <si>
+    <t>Avoid recreating List&lt;Triangle&gt; and clear()</t>
   </si>
 </sst>
 </file>
@@ -5410,7 +5416,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
@@ -5461,7 +5467,7 @@
         <v>60.127000000000002</v>
       </c>
       <c r="G2" s="44">
-        <f>D2/F2</f>
+        <f t="shared" ref="G2:G7" si="0">D2/F2</f>
         <v>515.57536547640825</v>
       </c>
     </row>
@@ -5485,7 +5491,7 @@
         <v>61.098999999999997</v>
       </c>
       <c r="G3" s="44">
-        <f>D3/F3</f>
+        <f t="shared" si="0"/>
         <v>556.47391937674922</v>
       </c>
       <c r="H3" s="46">
@@ -5513,7 +5519,7 @@
         <v>61.256</v>
       </c>
       <c r="G4" s="44">
-        <f>D4/F4</f>
+        <f t="shared" si="0"/>
         <v>571.37260023507906</v>
       </c>
       <c r="H4" s="46">
@@ -5541,7 +5547,7 @@
         <v>60.558999999999997</v>
       </c>
       <c r="G5" s="44">
-        <f>D5/F5</f>
+        <f t="shared" si="0"/>
         <v>577.94877722551564</v>
       </c>
       <c r="H5" s="46">
@@ -5569,7 +5575,7 @@
         <v>60.640999999999998</v>
       </c>
       <c r="G6" s="44">
-        <f>D6/F6</f>
+        <f t="shared" si="0"/>
         <v>577.16726307283852</v>
       </c>
       <c r="H6" s="46">
@@ -5597,7 +5603,7 @@
         <v>60.548000000000002</v>
       </c>
       <c r="G7" s="48">
-        <f>D7/F7</f>
+        <f t="shared" si="0"/>
         <v>578.05377551694517</v>
       </c>
       <c r="H7" s="49">
@@ -5615,10 +5621,34 @@
       <c r="C8" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F8" s="45"/>
+      <c r="D8">
+        <v>36000</v>
+      </c>
+      <c r="E8">
+        <v>0.70816066147017598</v>
+      </c>
+      <c r="F8" s="45">
+        <v>60.484999999999999</v>
+      </c>
+      <c r="G8" s="44">
+        <f t="shared" ref="G8" si="1">D8/F8</f>
+        <v>595.1888898073903</v>
+      </c>
+      <c r="H8" s="46">
+        <f>(G8/$G$2)-1</f>
+        <v>0.15441685088545021</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="1"/>
+      <c r="A9" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" s="50" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="F9" s="45"/>
     </row>
     <row r="10" spans="1:8">

</xml_diff>

<commit_message>
Working isosceles 4 triangles per square version
</commit_message>
<xml_diff>
--- a/src/main/resources/benchmarks.xlsx
+++ b/src/main/resources/benchmarks.xlsx
@@ -5568,7 +5568,7 @@
         <v>556.47391937674922</v>
       </c>
       <c r="I3" s="46">
-        <f>(H3/$H$2)-1</f>
+        <f t="shared" ref="I3:I8" si="1">(H3/$H$2)-1</f>
         <v>7.9326043560187243E-2</v>
       </c>
     </row>
@@ -5599,7 +5599,7 @@
         <v>571.37260023507906</v>
       </c>
       <c r="I4" s="46">
-        <f>(H4/$H$2)-1</f>
+        <f t="shared" si="1"/>
         <v>0.10822323659143862</v>
       </c>
     </row>
@@ -5630,7 +5630,7 @@
         <v>577.94877722551564</v>
       </c>
       <c r="I5" s="46">
-        <f>(H5/$H$2)-1</f>
+        <f t="shared" si="1"/>
         <v>0.12097826220124452</v>
       </c>
     </row>
@@ -5661,7 +5661,7 @@
         <v>577.16726307283852</v>
       </c>
       <c r="I6" s="46">
-        <f>(H6/$H$2)-1</f>
+        <f t="shared" si="1"/>
         <v>0.11946245247679244</v>
       </c>
     </row>
@@ -5692,7 +5692,7 @@
         <v>578.05377551694517</v>
       </c>
       <c r="I7" s="49">
-        <f>(H7/$H$2)-1</f>
+        <f t="shared" si="1"/>
         <v>0.12118191485507612</v>
       </c>
     </row>
@@ -5723,7 +5723,7 @@
         <v>595.1888898073903</v>
       </c>
       <c r="I8" s="57">
-        <f>(H8/$H$2)-1</f>
+        <f t="shared" si="1"/>
         <v>0.15441685088545021</v>
       </c>
     </row>
@@ -5750,7 +5750,7 @@
         <v>63.067</v>
       </c>
       <c r="H9" s="44">
-        <f t="shared" ref="H9:H10" si="1">E9/G9</f>
+        <f t="shared" ref="H9:H10" si="2">E9/G9</f>
         <v>79.280764900819761</v>
       </c>
       <c r="I9" s="46"/>
@@ -5778,7 +5778,7 @@
         <v>60.56</v>
       </c>
       <c r="H10" s="44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>66.050198150594454</v>
       </c>
       <c r="I10" s="46">
@@ -5807,7 +5807,7 @@
         <v>63.008000000000003</v>
       </c>
       <c r="H11" s="44">
-        <f t="shared" ref="H11" si="2">E11/G11</f>
+        <f t="shared" ref="H11" si="3">E11/G11</f>
         <v>79.355002539360072</v>
       </c>
       <c r="I11" s="46">
@@ -5836,7 +5836,7 @@
         <v>45199.45</v>
       </c>
       <c r="H12" s="44">
-        <f t="shared" ref="H12" si="3">E12/G12</f>
+        <f t="shared" ref="H12" si="4">E12/G12</f>
         <v>65.97425411149915</v>
       </c>
       <c r="I12" s="46">
@@ -5867,7 +5867,7 @@
         <v>2640.1689999999999</v>
       </c>
       <c r="H13" s="44">
-        <f t="shared" ref="H13" si="4">E13/G13</f>
+        <f t="shared" ref="H13" si="5">E13/G13</f>
         <v>143.55141659492253</v>
       </c>
       <c r="I13" s="46">

</xml_diff>

<commit_message>
Multithread but doesn't collaborate
</commit_message>
<xml_diff>
--- a/src/main/resources/benchmarks.xlsx
+++ b/src/main/resources/benchmarks.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17730" firstSheet="5" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17730" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -11514,7 +11514,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="G28" sqref="G28"/>
     </sheetView>
@@ -11559,7 +11559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Preparing for first real drawing ever
</commit_message>
<xml_diff>
--- a/src/main/resources/benchmarks.xlsx
+++ b/src/main/resources/benchmarks.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17730" firstSheet="5" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17730" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -981,6 +981,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11514,7 +11515,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="G28" sqref="G28"/>
     </sheetView>
@@ -11559,7 +11560,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>

</xml_diff>